<commit_message>
Added class NumPlayers and cleaned up main.p
</commit_message>
<xml_diff>
--- a/ofcroyalties.xlsx
+++ b/ofcroyalties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsr14\PycharmProjects\OFC-Royalty-Calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCC7976-89B7-46CF-8DFB-C93F1A549CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49812FD1-3CB4-489D-931D-03EB4DF52BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6270" yWindow="1020" windowWidth="21600" windowHeight="11385" xr2:uid="{BDF9B048-8EB2-4753-8D85-3AE9E78220FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>BOTTOM HAND</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Trip Aces</t>
+  </si>
+  <si>
+    <t>MIDDLE HAND-LOWBALL</t>
+  </si>
+  <si>
+    <t>Nine Low</t>
+  </si>
+  <si>
+    <t>Eight Low</t>
+  </si>
+  <si>
+    <t>Seven Low</t>
+  </si>
+  <si>
+    <t>Wheel</t>
   </si>
 </sst>
 </file>
@@ -490,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C138CACD-9F6F-4DAA-BFEB-FA5B4257B868}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,9 +516,11 @@
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,8 +530,11 @@
       <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -533,8 +553,14 @@
       <c r="J3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -553,8 +579,14 @@
       <c r="J4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -573,8 +605,14 @@
       <c r="J5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -593,8 +631,14 @@
       <c r="J6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -613,8 +657,14 @@
       <c r="J7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -634,7 +684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -654,7 +704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
@@ -668,7 +718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I11" s="1" t="s">
         <v>19</v>
       </c>
@@ -676,7 +726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I12" s="1" t="s">
         <v>20</v>
       </c>
@@ -684,7 +734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I13" s="1" t="s">
         <v>21</v>
       </c>
@@ -692,7 +742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I14" s="1" t="s">
         <v>22</v>
       </c>
@@ -700,7 +750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I15" s="1" t="s">
         <v>23</v>
       </c>
@@ -708,7 +758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I16" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
added all options to select boxes
</commit_message>
<xml_diff>
--- a/ofcroyalties.xlsx
+++ b/ofcroyalties.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsr14\PycharmProjects\OFC-Royalty-Calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49812FD1-3CB4-489D-931D-03EB4DF52BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111A0C4A-CD35-47B6-BC54-44C6690BCE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="1020" windowWidth="21600" windowHeight="11385" xr2:uid="{BDF9B048-8EB2-4753-8D85-3AE9E78220FB}"/>
+    <workbookView xWindow="3240" yWindow="1200" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{BDF9B048-8EB2-4753-8D85-3AE9E78220FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BottomHand" sheetId="1" r:id="rId1"/>
+    <sheet name="MiddleHand" sheetId="2" r:id="rId2"/>
+    <sheet name="TopHand" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
-  <si>
-    <t>BOTTOM HAND</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>HAND VALUE</t>
   </si>
@@ -60,18 +59,12 @@
     <t>Royal Flush</t>
   </si>
   <si>
-    <t>MIDDLE HAND</t>
-  </si>
-  <si>
     <t>UNITS</t>
   </si>
   <si>
     <t>Set</t>
   </si>
   <si>
-    <t>TOP HAND</t>
-  </si>
-  <si>
     <t>Sixes</t>
   </si>
   <si>
@@ -136,9 +129,6 @@
   </si>
   <si>
     <t>Trip Aces</t>
-  </si>
-  <si>
-    <t>MIDDLE HAND-LOWBALL</t>
   </si>
   <si>
     <t>Nine Low</t>
@@ -505,11 +495,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C138CACD-9F6F-4DAA-BFEB-FA5B4257B868}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -520,321 +508,377 @@
     <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D6265C-2612-43AB-A554-F38AD7ECA416}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>4</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="1">
-        <v>2</v>
-      </c>
-      <c r="L5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1">
-        <v>8</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="1">
-        <v>3</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="1">
-        <v>4</v>
-      </c>
-      <c r="L7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E6AAB9-7578-4E46-B120-7AF48948FD10}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1">
         <v>16</v>
       </c>
-      <c r="J8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1">
-        <v>50</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J22" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J23" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J24" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="B23" s="1">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaned up classes, put hand vals into a variable
</commit_message>
<xml_diff>
--- a/ofcroyalties.xlsx
+++ b/ofcroyalties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsr14\PycharmProjects\OFC-Royalty-Calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111A0C4A-CD35-47B6-BC54-44C6690BCE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD9C345-1ADE-43E3-A6BD-5959EEAC85AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="1200" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{BDF9B048-8EB2-4753-8D85-3AE9E78220FB}"/>
+    <workbookView xWindow="29250" yWindow="1230" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{BDF9B048-8EB2-4753-8D85-3AE9E78220FB}"/>
   </bookViews>
   <sheets>
     <sheet name="BottomHand" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>HAND VALUE</t>
   </si>
@@ -47,100 +47,106 @@
     <t>Flush</t>
   </si>
   <si>
-    <t>Full House</t>
-  </si>
-  <si>
     <t>Quads</t>
   </si>
   <si>
-    <t>Straight Flush</t>
-  </si>
-  <si>
-    <t>Royal Flush</t>
-  </si>
-  <si>
     <t>UNITS</t>
   </si>
   <si>
     <t>Set</t>
   </si>
   <si>
+    <t>Eights</t>
+  </si>
+  <si>
+    <t>Nines</t>
+  </si>
+  <si>
+    <t>Tens</t>
+  </si>
+  <si>
+    <t>Jacks</t>
+  </si>
+  <si>
+    <t>Queens</t>
+  </si>
+  <si>
+    <t>Kings</t>
+  </si>
+  <si>
+    <t>Aces</t>
+  </si>
+  <si>
+    <t>Wheel</t>
+  </si>
+  <si>
+    <t>Non-Scoring Hand</t>
+  </si>
+  <si>
+    <t>Trip-Deuces</t>
+  </si>
+  <si>
+    <t>Trip-Threes</t>
+  </si>
+  <si>
+    <t>Trip-Fours</t>
+  </si>
+  <si>
+    <t>Trip-Fives</t>
+  </si>
+  <si>
+    <t>Trip-Sixes</t>
+  </si>
+  <si>
+    <t>Trip-Sevens</t>
+  </si>
+  <si>
+    <t>Trip-Eights</t>
+  </si>
+  <si>
+    <t>Trip-Nines</t>
+  </si>
+  <si>
+    <t>Trip-Tens</t>
+  </si>
+  <si>
+    <t>Trip-Jacks</t>
+  </si>
+  <si>
+    <t>Trip-Queens</t>
+  </si>
+  <si>
+    <t>Trip-Kings</t>
+  </si>
+  <si>
+    <t>Trip-Aces</t>
+  </si>
+  <si>
+    <t>Full-House</t>
+  </si>
+  <si>
+    <t>Straight-Flush</t>
+  </si>
+  <si>
+    <t>Royal-Flush</t>
+  </si>
+  <si>
+    <t>Nine-Low</t>
+  </si>
+  <si>
+    <t>Eight-Low</t>
+  </si>
+  <si>
+    <t>Seven-Low</t>
+  </si>
+  <si>
+    <t>Non-Scoring</t>
+  </si>
+  <si>
     <t>Sixes</t>
   </si>
   <si>
     <t>Sevens</t>
-  </si>
-  <si>
-    <t>Eights</t>
-  </si>
-  <si>
-    <t>Nines</t>
-  </si>
-  <si>
-    <t>Tens</t>
-  </si>
-  <si>
-    <t>Jacks</t>
-  </si>
-  <si>
-    <t>Queens</t>
-  </si>
-  <si>
-    <t>Kings</t>
-  </si>
-  <si>
-    <t>Aces</t>
-  </si>
-  <si>
-    <t>Trip Deuces</t>
-  </si>
-  <si>
-    <t>Trip Threes</t>
-  </si>
-  <si>
-    <t>Trip Fours</t>
-  </si>
-  <si>
-    <t>Trip Fives</t>
-  </si>
-  <si>
-    <t>Trip Sixes</t>
-  </si>
-  <si>
-    <t>Trip Sevens</t>
-  </si>
-  <si>
-    <t>Trip Eights</t>
-  </si>
-  <si>
-    <t>Trip Nines</t>
-  </si>
-  <si>
-    <t>Trip Tens</t>
-  </si>
-  <si>
-    <t>Trip Jacks</t>
-  </si>
-  <si>
-    <t>Trip Queens</t>
-  </si>
-  <si>
-    <t>Trip Kings</t>
-  </si>
-  <si>
-    <t>Trip Aces</t>
-  </si>
-  <si>
-    <t>Nine Low</t>
-  </si>
-  <si>
-    <t>Eight Low</t>
-  </si>
-  <si>
-    <t>Seven Low</t>
-  </si>
-  <si>
-    <t>Wheel</t>
   </si>
 </sst>
 </file>
@@ -176,10 +182,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,13 +507,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C138CACD-9F6F-4DAA-BFEB-FA5B4257B868}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" customWidth="1"/>
@@ -513,56 +527,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
         <v>25</v>
       </c>
     </row>
@@ -573,15 +595,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D6265C-2612-43AB-A554-F38AD7ECA416}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -589,94 +611,102 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1">
         <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
         <v>8</v>
       </c>
     </row>
@@ -687,15 +717,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E6AAB9-7578-4E46-B120-7AF48948FD10}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -703,186 +735,195 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1">
-        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>